<commit_message>
Minor Correction - removed extraneous data
</commit_message>
<xml_diff>
--- a/COMCRD.BOM.xlsx
+++ b/COMCRD.BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Product Name: Command Card</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Design by Codeshelf, Printed by Kinko's</t>
-  </si>
-  <si>
-    <t>Part not listed on website; contact Lois Buckner loisb@quantumstorage.com</t>
   </si>
   <si>
     <t>Command Update Decal</t>
@@ -113,8 +110,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="6">
@@ -208,77 +205,81 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -301,203 +302,203 @@
   <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.6925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.2851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.0814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.5407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.7148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.5777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="79.9185185185185"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.8037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.49259259259259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.5703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="53.3333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.0592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.1777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.562962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="86.6518518518518"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.9592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.2703703703704"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" s="5" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="7" t="n">
         <v>42272</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="11" t="n">
+      <c r="F3" s="10" t="n">
         <v>42276</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" s="15" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" s="14" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="47.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8" t="n">
+      <c r="E6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7" t="n">
         <v>42272</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>42272</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8" t="n">
+      <c r="C8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7" t="n">
         <v>42272</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="8" t="n">
-        <v>42272</v>
-      </c>
-      <c r="G8" s="17" t="s">
+      <c r="H8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="11" t="n">
+      <c r="F9" s="10" t="n">
         <v>42276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Minor Correction - Release IDs
</commit_message>
<xml_diff>
--- a/COMCRD.BOM.xlsx
+++ b/COMCRD.BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Product Name: Command Card</t>
   </si>
@@ -23,49 +23,52 @@
     <t>Tag:</t>
   </si>
   <si>
+    <t>COMCRD v1.0</t>
+  </si>
+  <si>
+    <t>Product Number: COMCRD v1.0</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t>Last Updated:</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Drawing/Part No.</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Command Card</t>
+  </si>
+  <si>
+    <t>Trifold scannable command card, laminated</t>
+  </si>
+  <si>
     <t>COMCRD</t>
-  </si>
-  <si>
-    <t>Product Number: COMCRD</t>
-  </si>
-  <si>
-    <t>Date:</t>
-  </si>
-  <si>
-    <t>Last Updated:</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Drawing/Part No.</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Command Card</t>
-  </si>
-  <si>
-    <t>Trifold scannable command card, laminated</t>
   </si>
   <si>
     <t>Design by Codeshelf, Printed by Kinko's</t>
@@ -114,7 +117,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -146,6 +149,14 @@
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="16"/>
+      <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -180,7 +191,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,8 +215,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,6 +288,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -283,13 +301,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -302,21 +321,21 @@
   <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.5703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="53.3333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.0592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.1777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.562962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="86.6518518518518"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.9592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="10.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.9666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="59.3777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="62.6555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="30.5555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.9740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="27.7074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.4444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="101.755555555556"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.7111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="11.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -419,7 +438,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>1</v>
@@ -428,32 +447,32 @@
         <v>42272</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="A7" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="C7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="D7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="19" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="7" t="n">
         <v>42272</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>17</v>
+      <c r="G7" s="18" t="s">
+        <v>18</v>
       </c>
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
@@ -463,13 +482,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" s="9" t="n">
         <v>1</v>
@@ -478,25 +497,25 @@
         <v>42272</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="n">
+      <c r="A9" s="18" t="n">
         <v>2</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="C9" s="18" t="s">
         <v>28</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="F9" s="10" t="n">
         <v>42276</v>
@@ -524,7 +543,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;"Arial,Regular"LEDCON.MECH.BOM</oddHeader>
+    <oddHeader>&amp;L&amp;"Arial,Regular"COMCRD.BOM</oddHeader>
     <oddFooter>&amp;L&amp;"Arial,Regular"	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>